<commit_message>
fix: resolve bug when inputting supervisor lecturer
</commit_message>
<xml_diff>
--- a/public/templates/logbook-template.xlsx
+++ b/public/templates/logbook-template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adhie\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\logbook-generator\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82562F8E-BF3C-4F9B-B647-F61319731BE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE1EDC83-B33B-4844-9C29-CBEDBF76F490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Waktu</t>
   </si>
@@ -72,12 +72,6 @@
     <t>Dosen</t>
   </si>
   <si>
-    <t>files/bukti1.pdf</t>
-  </si>
-  <si>
-    <t>files/bukti2.png</t>
-  </si>
-  <si>
     <t>IPB University</t>
   </si>
   <si>
@@ -85,6 +79,9 @@
   </si>
   <si>
     <t>Studi literatur terkait kerabat hewan ambalabu</t>
+  </si>
+  <si>
+    <t>1,2</t>
   </si>
 </sst>
 </file>
@@ -483,7 +480,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="77" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomLeft" activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -543,17 +540,15 @@
         <v>1</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H2" s="6">
         <v>1</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
@@ -572,17 +567,15 @@
         <v>0</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="6">
-        <v>1.2</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="H3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>

</xml_diff>

<commit_message>
add multiple result download type
</commit_message>
<xml_diff>
--- a/public/templates/logbook-template.xlsx
+++ b/public/templates/logbook-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adhie\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82562F8E-BF3C-4F9B-B647-F61319731BE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F8C1ED7-BBAE-4C58-A2DA-CCF8BA348995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>Waktu</t>
   </si>
@@ -66,9 +66,6 @@
     <t>16:00</t>
   </si>
   <si>
-    <t>26/08/2025</t>
-  </si>
-  <si>
     <t>Dosen</t>
   </si>
   <si>
@@ -85,12 +82,24 @@
   </si>
   <si>
     <t>Studi literatur terkait kerabat hewan ambalabu</t>
+  </si>
+  <si>
+    <t>Kenapa hebat?</t>
+  </si>
+  <si>
+    <t>files/bukti1.png</t>
+  </si>
+  <si>
+    <t>0, 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="[$-13809]hh:mm;@"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -103,6 +112,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -151,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -171,12 +181,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="166" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,15 +505,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="77" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="3" width="10" customWidth="1"/>
+    <col min="1" max="1" width="16.44140625" style="14" customWidth="1"/>
+    <col min="2" max="3" width="10" style="11" customWidth="1"/>
     <col min="4" max="5" width="12" customWidth="1"/>
     <col min="6" max="6" width="36.88671875" customWidth="1"/>
     <col min="7" max="7" width="65.77734375" customWidth="1"/>
@@ -498,13 +522,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -520,85 +544,103 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="7">
+        <v>45832</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="9" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="6">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7">
+        <v>45833</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
+        <v>45834</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2">
         <v>3</v>
       </c>
-      <c r="E2" s="2">
-        <v>1</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="6">
-        <v>1</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8">
-        <v>46261</v>
-      </c>
-      <c r="B3" s="7">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="C3" s="7">
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="D3" s="2">
-        <v>3</v>
-      </c>
-      <c r="E3" s="2">
+      <c r="E4" s="2">
+        <v>2</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="6">
         <v>0</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="6">
-        <v>1.2</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
+      <c r="I4" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="5" spans="1:9" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -607,9 +649,9 @@
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -618,9 +660,9 @@
       <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:9" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -629,9 +671,9 @@
       <c r="I7" s="2"/>
     </row>
     <row r="8" spans="1:9" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -640,9 +682,9 @@
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:9" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -651,9 +693,9 @@
       <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:9" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -662,9 +704,9 @@
       <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:9" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -673,9 +715,9 @@
       <c r="I11" s="2"/>
     </row>
     <row r="12" spans="1:9" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -684,9 +726,9 @@
       <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:9" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -695,9 +737,9 @@
       <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:9" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -706,9 +748,9 @@
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:9" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
+      <c r="A15" s="7"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -717,9 +759,9 @@
       <c r="I15" s="2"/>
     </row>
     <row r="16" spans="1:9" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+      <c r="A16" s="7"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -728,9 +770,9 @@
       <c r="I16" s="2"/>
     </row>
     <row r="17" spans="1:9" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
@@ -739,9 +781,9 @@
       <c r="I17" s="2"/>
     </row>
     <row r="18" spans="1:9" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
+      <c r="A18" s="7"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -750,9 +792,9 @@
       <c r="I18" s="2"/>
     </row>
     <row r="19" spans="1:9" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
@@ -761,9 +803,9 @@
       <c r="I19" s="2"/>
     </row>
     <row r="20" spans="1:9" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -772,9 +814,9 @@
       <c r="I20" s="2"/>
     </row>
     <row r="21" spans="1:9" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
+      <c r="A21" s="7"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
@@ -783,9 +825,9 @@
       <c r="I21" s="2"/>
     </row>
     <row r="22" spans="1:9" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
+      <c r="A22" s="13"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="5"/>
@@ -793,9 +835,9 @@
       <c r="H22" s="4"/>
     </row>
     <row r="23" spans="1:9" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
+      <c r="A23" s="13"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="5"/>
@@ -803,9 +845,9 @@
       <c r="H23" s="4"/>
     </row>
     <row r="24" spans="1:9" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
+      <c r="A24" s="13"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="5"/>
@@ -813,9 +855,9 @@
       <c r="H24" s="4"/>
     </row>
     <row r="25" spans="1:9" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
+      <c r="A25" s="13"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="5"/>
@@ -823,9 +865,9 @@
       <c r="H25" s="4"/>
     </row>
     <row r="26" spans="1:9" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
+      <c r="A26" s="13"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="5"/>
@@ -833,9 +875,9 @@
       <c r="H26" s="4"/>
     </row>
     <row r="27" spans="1:9" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
+      <c r="A27" s="13"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="5"/>
@@ -843,9 +885,9 @@
       <c r="H27" s="4"/>
     </row>
     <row r="28" spans="1:9" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
+      <c r="A28" s="13"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="5"/>
@@ -853,9 +895,9 @@
       <c r="H28" s="4"/>
     </row>
     <row r="29" spans="1:9" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
+      <c r="A29" s="13"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="5"/>
@@ -863,9 +905,9 @@
       <c r="H29" s="4"/>
     </row>
     <row r="30" spans="1:9" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
+      <c r="A30" s="13"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="5"/>
@@ -873,9 +915,9 @@
       <c r="H30" s="4"/>
     </row>
     <row r="31" spans="1:9" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
+      <c r="A31" s="13"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="5"/>
@@ -883,9 +925,9 @@
       <c r="H31" s="4"/>
     </row>
     <row r="32" spans="1:9" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
+      <c r="A32" s="13"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="5"/>
@@ -893,9 +935,9 @@
       <c r="H32" s="4"/>
     </row>
     <row r="33" spans="1:8" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="4"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
+      <c r="A33" s="13"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="F33" s="5"/>
@@ -903,9 +945,9 @@
       <c r="H33" s="4"/>
     </row>
     <row r="34" spans="1:8" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
+      <c r="A34" s="13"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
       <c r="F34" s="5"/>
@@ -913,9 +955,9 @@
       <c r="H34" s="4"/>
     </row>
     <row r="35" spans="1:8" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
+      <c r="A35" s="13"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
       <c r="F35" s="5"/>
@@ -923,9 +965,9 @@
       <c r="H35" s="4"/>
     </row>
     <row r="36" spans="1:8" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
+      <c r="A36" s="13"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
       <c r="F36" s="5"/>
@@ -933,9 +975,9 @@
       <c r="H36" s="4"/>
     </row>
     <row r="37" spans="1:8" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
+      <c r="A37" s="13"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
       <c r="F37" s="5"/>
@@ -943,9 +985,9 @@
       <c r="H37" s="4"/>
     </row>
     <row r="38" spans="1:8" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="4"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
+      <c r="A38" s="13"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
       <c r="F38" s="5"/>
@@ -953,9 +995,9 @@
       <c r="H38" s="4"/>
     </row>
     <row r="39" spans="1:8" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="4"/>
-      <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
+      <c r="A39" s="13"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
       <c r="F39" s="5"/>
@@ -963,9 +1005,9 @@
       <c r="H39" s="4"/>
     </row>
     <row r="40" spans="1:8" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="4"/>
-      <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
+      <c r="A40" s="13"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
       <c r="F40" s="5"/>
@@ -973,9 +1015,9 @@
       <c r="H40" s="4"/>
     </row>
     <row r="41" spans="1:8" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="4"/>
-      <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
+      <c r="A41" s="13"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="10"/>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
       <c r="F41" s="5"/>
@@ -983,9 +1025,9 @@
       <c r="H41" s="4"/>
     </row>
     <row r="42" spans="1:8" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="4"/>
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
+      <c r="A42" s="13"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="10"/>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
       <c r="F42" s="5"/>
@@ -993,9 +1035,9 @@
       <c r="H42" s="4"/>
     </row>
     <row r="43" spans="1:8" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="4"/>
-      <c r="B43" s="4"/>
-      <c r="C43" s="4"/>
+      <c r="A43" s="13"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
       <c r="F43" s="5"/>
@@ -1003,9 +1045,9 @@
       <c r="H43" s="4"/>
     </row>
     <row r="44" spans="1:8" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="4"/>
-      <c r="B44" s="4"/>
-      <c r="C44" s="4"/>
+      <c r="A44" s="13"/>
+      <c r="B44" s="10"/>
+      <c r="C44" s="10"/>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
       <c r="F44" s="5"/>
@@ -1013,9 +1055,9 @@
       <c r="H44" s="4"/>
     </row>
     <row r="45" spans="1:8" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="4"/>
-      <c r="B45" s="4"/>
-      <c r="C45" s="4"/>
+      <c r="A45" s="13"/>
+      <c r="B45" s="10"/>
+      <c r="C45" s="10"/>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
       <c r="F45" s="5"/>
@@ -1023,9 +1065,9 @@
       <c r="H45" s="4"/>
     </row>
     <row r="46" spans="1:8" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="4"/>
-      <c r="B46" s="4"/>
-      <c r="C46" s="4"/>
+      <c r="A46" s="13"/>
+      <c r="B46" s="10"/>
+      <c r="C46" s="10"/>
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
       <c r="F46" s="5"/>
@@ -1033,9 +1075,9 @@
       <c r="H46" s="4"/>
     </row>
     <row r="47" spans="1:8" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="4"/>
-      <c r="B47" s="4"/>
-      <c r="C47" s="4"/>
+      <c r="A47" s="13"/>
+      <c r="B47" s="10"/>
+      <c r="C47" s="10"/>
       <c r="D47" s="4"/>
       <c r="E47" s="4"/>
       <c r="F47" s="5"/>
@@ -1043,9 +1085,9 @@
       <c r="H47" s="4"/>
     </row>
     <row r="48" spans="1:8" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="4"/>
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
+      <c r="A48" s="13"/>
+      <c r="B48" s="10"/>
+      <c r="C48" s="10"/>
       <c r="D48" s="4"/>
       <c r="E48" s="4"/>
       <c r="F48" s="5"/>
@@ -1053,9 +1095,9 @@
       <c r="H48" s="4"/>
     </row>
     <row r="49" spans="1:8" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="4"/>
-      <c r="B49" s="4"/>
-      <c r="C49" s="4"/>
+      <c r="A49" s="13"/>
+      <c r="B49" s="10"/>
+      <c r="C49" s="10"/>
       <c r="D49" s="4"/>
       <c r="E49" s="4"/>
       <c r="F49" s="5"/>
@@ -1063,9 +1105,9 @@
       <c r="H49" s="4"/>
     </row>
     <row r="50" spans="1:8" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="4"/>
-      <c r="B50" s="4"/>
-      <c r="C50" s="4"/>
+      <c r="A50" s="13"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="10"/>
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
       <c r="F50" s="5"/>
@@ -1073,9 +1115,9 @@
       <c r="H50" s="4"/>
     </row>
     <row r="51" spans="1:8" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="4"/>
-      <c r="B51" s="4"/>
-      <c r="C51" s="4"/>
+      <c r="A51" s="13"/>
+      <c r="B51" s="10"/>
+      <c r="C51" s="10"/>
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
       <c r="F51" s="5"/>
@@ -1083,9 +1125,9 @@
       <c r="H51" s="4"/>
     </row>
     <row r="52" spans="1:8" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="4"/>
-      <c r="B52" s="4"/>
-      <c r="C52" s="4"/>
+      <c r="A52" s="13"/>
+      <c r="B52" s="10"/>
+      <c r="C52" s="10"/>
       <c r="D52" s="4"/>
       <c r="E52" s="4"/>
       <c r="F52" s="5"/>
@@ -1093,9 +1135,9 @@
       <c r="H52" s="4"/>
     </row>
     <row r="53" spans="1:8" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="4"/>
-      <c r="B53" s="4"/>
-      <c r="C53" s="4"/>
+      <c r="A53" s="13"/>
+      <c r="B53" s="10"/>
+      <c r="C53" s="10"/>
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
       <c r="F53" s="5"/>
@@ -1103,9 +1145,9 @@
       <c r="H53" s="4"/>
     </row>
     <row r="54" spans="1:8" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="4"/>
-      <c r="B54" s="4"/>
-      <c r="C54" s="4"/>
+      <c r="A54" s="13"/>
+      <c r="B54" s="10"/>
+      <c r="C54" s="10"/>
       <c r="D54" s="4"/>
       <c r="E54" s="4"/>
       <c r="F54" s="5"/>
@@ -1113,9 +1155,9 @@
       <c r="H54" s="4"/>
     </row>
     <row r="55" spans="1:8" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="4"/>
-      <c r="B55" s="4"/>
-      <c r="C55" s="4"/>
+      <c r="A55" s="13"/>
+      <c r="B55" s="10"/>
+      <c r="C55" s="10"/>
       <c r="D55" s="4"/>
       <c r="E55" s="4"/>
       <c r="F55" s="5"/>
@@ -1123,9 +1165,9 @@
       <c r="H55" s="4"/>
     </row>
     <row r="56" spans="1:8" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="4"/>
-      <c r="B56" s="4"/>
-      <c r="C56" s="4"/>
+      <c r="A56" s="13"/>
+      <c r="B56" s="10"/>
+      <c r="C56" s="10"/>
       <c r="D56" s="4"/>
       <c r="E56" s="4"/>
       <c r="F56" s="5"/>
@@ -1133,9 +1175,9 @@
       <c r="H56" s="4"/>
     </row>
     <row r="57" spans="1:8" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="4"/>
-      <c r="B57" s="4"/>
-      <c r="C57" s="4"/>
+      <c r="A57" s="13"/>
+      <c r="B57" s="10"/>
+      <c r="C57" s="10"/>
       <c r="D57" s="4"/>
       <c r="E57" s="4"/>
       <c r="F57" s="5"/>
@@ -1143,9 +1185,9 @@
       <c r="H57" s="4"/>
     </row>
     <row r="58" spans="1:8" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="4"/>
-      <c r="B58" s="4"/>
-      <c r="C58" s="4"/>
+      <c r="A58" s="13"/>
+      <c r="B58" s="10"/>
+      <c r="C58" s="10"/>
       <c r="D58" s="4"/>
       <c r="E58" s="4"/>
       <c r="F58" s="5"/>
@@ -1153,9 +1195,9 @@
       <c r="H58" s="4"/>
     </row>
     <row r="59" spans="1:8" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="4"/>
-      <c r="B59" s="4"/>
-      <c r="C59" s="4"/>
+      <c r="A59" s="13"/>
+      <c r="B59" s="10"/>
+      <c r="C59" s="10"/>
       <c r="D59" s="4"/>
       <c r="E59" s="4"/>
       <c r="F59" s="5"/>
@@ -1163,9 +1205,9 @@
       <c r="H59" s="4"/>
     </row>
     <row r="60" spans="1:8" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="4"/>
-      <c r="B60" s="4"/>
-      <c r="C60" s="4"/>
+      <c r="A60" s="13"/>
+      <c r="B60" s="10"/>
+      <c r="C60" s="10"/>
       <c r="D60" s="4"/>
       <c r="E60" s="4"/>
       <c r="F60" s="5"/>
@@ -1173,9 +1215,9 @@
       <c r="H60" s="4"/>
     </row>
     <row r="61" spans="1:8" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="4"/>
-      <c r="B61" s="4"/>
-      <c r="C61" s="4"/>
+      <c r="A61" s="13"/>
+      <c r="B61" s="10"/>
+      <c r="C61" s="10"/>
       <c r="D61" s="4"/>
       <c r="E61" s="4"/>
       <c r="F61" s="5"/>
@@ -1183,9 +1225,9 @@
       <c r="H61" s="4"/>
     </row>
     <row r="62" spans="1:8" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="4"/>
-      <c r="B62" s="4"/>
-      <c r="C62" s="4"/>
+      <c r="A62" s="13"/>
+      <c r="B62" s="10"/>
+      <c r="C62" s="10"/>
       <c r="D62" s="4"/>
       <c r="E62" s="4"/>
       <c r="F62" s="5"/>
@@ -1193,9 +1235,9 @@
       <c r="H62" s="4"/>
     </row>
     <row r="63" spans="1:8" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="4"/>
-      <c r="B63" s="4"/>
-      <c r="C63" s="4"/>
+      <c r="A63" s="13"/>
+      <c r="B63" s="10"/>
+      <c r="C63" s="10"/>
       <c r="D63" s="4"/>
       <c r="E63" s="4"/>
       <c r="F63" s="5"/>
@@ -1203,9 +1245,9 @@
       <c r="H63" s="4"/>
     </row>
     <row r="64" spans="1:8" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="4"/>
-      <c r="B64" s="4"/>
-      <c r="C64" s="4"/>
+      <c r="A64" s="13"/>
+      <c r="B64" s="10"/>
+      <c r="C64" s="10"/>
       <c r="D64" s="4"/>
       <c r="E64" s="4"/>
       <c r="F64" s="5"/>
@@ -1213,9 +1255,9 @@
       <c r="H64" s="4"/>
     </row>
     <row r="65" spans="1:8" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="4"/>
-      <c r="B65" s="4"/>
-      <c r="C65" s="4"/>
+      <c r="A65" s="13"/>
+      <c r="B65" s="10"/>
+      <c r="C65" s="10"/>
       <c r="D65" s="4"/>
       <c r="E65" s="4"/>
       <c r="F65" s="5"/>
@@ -1223,9 +1265,9 @@
       <c r="H65" s="4"/>
     </row>
     <row r="66" spans="1:8" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="4"/>
-      <c r="B66" s="4"/>
-      <c r="C66" s="4"/>
+      <c r="A66" s="13"/>
+      <c r="B66" s="10"/>
+      <c r="C66" s="10"/>
       <c r="D66" s="4"/>
       <c r="E66" s="4"/>
       <c r="F66" s="5"/>
@@ -1233,9 +1275,9 @@
       <c r="H66" s="4"/>
     </row>
     <row r="67" spans="1:8" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="4"/>
-      <c r="B67" s="4"/>
-      <c r="C67" s="4"/>
+      <c r="A67" s="13"/>
+      <c r="B67" s="10"/>
+      <c r="C67" s="10"/>
       <c r="D67" s="4"/>
       <c r="E67" s="4"/>
       <c r="F67" s="5"/>
@@ -1243,9 +1285,9 @@
       <c r="H67" s="4"/>
     </row>
     <row r="68" spans="1:8" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="4"/>
-      <c r="B68" s="4"/>
-      <c r="C68" s="4"/>
+      <c r="A68" s="13"/>
+      <c r="B68" s="10"/>
+      <c r="C68" s="10"/>
       <c r="D68" s="4"/>
       <c r="E68" s="4"/>
       <c r="F68" s="5"/>
@@ -1253,9 +1295,9 @@
       <c r="H68" s="4"/>
     </row>
     <row r="69" spans="1:8" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="4"/>
-      <c r="B69" s="4"/>
-      <c r="C69" s="4"/>
+      <c r="A69" s="13"/>
+      <c r="B69" s="10"/>
+      <c r="C69" s="10"/>
       <c r="D69" s="4"/>
       <c r="E69" s="4"/>
       <c r="F69" s="5"/>
@@ -1263,9 +1305,9 @@
       <c r="H69" s="4"/>
     </row>
     <row r="70" spans="1:8" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="4"/>
-      <c r="B70" s="4"/>
-      <c r="C70" s="4"/>
+      <c r="A70" s="13"/>
+      <c r="B70" s="10"/>
+      <c r="C70" s="10"/>
       <c r="D70" s="4"/>
       <c r="E70" s="4"/>
       <c r="F70" s="5"/>
@@ -1273,9 +1315,9 @@
       <c r="H70" s="4"/>
     </row>
     <row r="71" spans="1:8" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="4"/>
-      <c r="B71" s="4"/>
-      <c r="C71" s="4"/>
+      <c r="A71" s="13"/>
+      <c r="B71" s="10"/>
+      <c r="C71" s="10"/>
       <c r="D71" s="4"/>
       <c r="E71" s="4"/>
       <c r="F71" s="5"/>
@@ -1283,9 +1325,9 @@
       <c r="H71" s="4"/>
     </row>
     <row r="72" spans="1:8" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="4"/>
-      <c r="B72" s="4"/>
-      <c r="C72" s="4"/>
+      <c r="A72" s="13"/>
+      <c r="B72" s="10"/>
+      <c r="C72" s="10"/>
       <c r="D72" s="4"/>
       <c r="E72" s="4"/>
       <c r="F72" s="5"/>
@@ -1293,9 +1335,9 @@
       <c r="H72" s="4"/>
     </row>
     <row r="73" spans="1:8" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="4"/>
-      <c r="B73" s="4"/>
-      <c r="C73" s="4"/>
+      <c r="A73" s="13"/>
+      <c r="B73" s="10"/>
+      <c r="C73" s="10"/>
       <c r="D73" s="4"/>
       <c r="E73" s="4"/>
       <c r="F73" s="5"/>
@@ -1303,9 +1345,9 @@
       <c r="H73" s="4"/>
     </row>
     <row r="74" spans="1:8" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="4"/>
-      <c r="B74" s="4"/>
-      <c r="C74" s="4"/>
+      <c r="A74" s="13"/>
+      <c r="B74" s="10"/>
+      <c r="C74" s="10"/>
       <c r="D74" s="4"/>
       <c r="E74" s="4"/>
       <c r="F74" s="5"/>
@@ -1313,9 +1355,9 @@
       <c r="H74" s="4"/>
     </row>
     <row r="75" spans="1:8" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="4"/>
-      <c r="B75" s="4"/>
-      <c r="C75" s="4"/>
+      <c r="A75" s="13"/>
+      <c r="B75" s="10"/>
+      <c r="C75" s="10"/>
       <c r="D75" s="4"/>
       <c r="E75" s="4"/>
       <c r="F75" s="5"/>
@@ -1323,9 +1365,9 @@
       <c r="H75" s="4"/>
     </row>
     <row r="76" spans="1:8" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="4"/>
-      <c r="B76" s="4"/>
-      <c r="C76" s="4"/>
+      <c r="A76" s="13"/>
+      <c r="B76" s="10"/>
+      <c r="C76" s="10"/>
       <c r="D76" s="4"/>
       <c r="E76" s="4"/>
       <c r="F76" s="5"/>
@@ -1333,9 +1375,9 @@
       <c r="H76" s="4"/>
     </row>
     <row r="77" spans="1:8" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="4"/>
-      <c r="B77" s="4"/>
-      <c r="C77" s="4"/>
+      <c r="A77" s="13"/>
+      <c r="B77" s="10"/>
+      <c r="C77" s="10"/>
       <c r="D77" s="4"/>
       <c r="E77" s="4"/>
       <c r="F77" s="5"/>
@@ -1343,9 +1385,9 @@
       <c r="H77" s="4"/>
     </row>
     <row r="78" spans="1:8" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="4"/>
-      <c r="B78" s="4"/>
-      <c r="C78" s="4"/>
+      <c r="A78" s="13"/>
+      <c r="B78" s="10"/>
+      <c r="C78" s="10"/>
       <c r="D78" s="4"/>
       <c r="E78" s="4"/>
       <c r="F78" s="5"/>
@@ -1353,9 +1395,9 @@
       <c r="H78" s="4"/>
     </row>
     <row r="79" spans="1:8" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="4"/>
-      <c r="B79" s="4"/>
-      <c r="C79" s="4"/>
+      <c r="A79" s="13"/>
+      <c r="B79" s="10"/>
+      <c r="C79" s="10"/>
       <c r="D79" s="4"/>
       <c r="E79" s="4"/>
       <c r="F79" s="5"/>
@@ -1363,9 +1405,9 @@
       <c r="H79" s="4"/>
     </row>
     <row r="80" spans="1:8" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="4"/>
-      <c r="B80" s="4"/>
-      <c r="C80" s="4"/>
+      <c r="A80" s="13"/>
+      <c r="B80" s="10"/>
+      <c r="C80" s="10"/>
       <c r="D80" s="4"/>
       <c r="E80" s="4"/>
       <c r="F80" s="5"/>
@@ -1373,9 +1415,9 @@
       <c r="H80" s="4"/>
     </row>
     <row r="81" spans="1:8" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="4"/>
-      <c r="B81" s="4"/>
-      <c r="C81" s="4"/>
+      <c r="A81" s="13"/>
+      <c r="B81" s="10"/>
+      <c r="C81" s="10"/>
       <c r="D81" s="4"/>
       <c r="E81" s="4"/>
       <c r="F81" s="5"/>
@@ -1385,6 +1427,14 @@
   </sheetData>
   <autoFilter ref="A1:G81" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
+  <dataValidations count="2">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D2:D21" xr:uid="{43AB4E7C-3B5B-4B6D-89C6-F560D1C88627}">
+      <formula1>"1,2,3"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E2:E21" xr:uid="{B8EF64A4-AAA4-4D88-ADA6-6DBE61AC482A}">
+      <formula1>"0,1,2"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: validation error on login, file upload, and dosen fields
</commit_message>
<xml_diff>
--- a/public/templates/logbook-template.xlsx
+++ b/public/templates/logbook-template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adhie\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adhie\Downloads\logbook-package-example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F8C1ED7-BBAE-4C58-A2DA-CCF8BA348995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80743DDF-230F-4A93-9E76-473073724452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>Waktu</t>
   </si>
@@ -88,9 +88,6 @@
   </si>
   <si>
     <t>files/bukti1.png</t>
-  </si>
-  <si>
-    <t>0, 1</t>
   </si>
 </sst>
 </file>
@@ -98,7 +95,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-13809]hh:mm;@"/>
+    <numFmt numFmtId="164" formatCode="[$-13809]hh:mm;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -184,16 +181,16 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -507,7 +504,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -573,7 +570,7 @@
         <v>14</v>
       </c>
       <c r="H2" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>11</v>
@@ -601,8 +598,8 @@
       <c r="G3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="6" t="s">
-        <v>18</v>
+      <c r="H3" s="6">
+        <v>1.2</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>12</v>
@@ -631,7 +628,7 @@
         <v>16</v>
       </c>
       <c r="H4" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
fix: time and date format behavior
</commit_message>
<xml_diff>
--- a/public/templates/logbook-template.xlsx
+++ b/public/templates/logbook-template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adhie\Downloads\Test File\logbook-package-example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Perkuliahan\CodingLife\0_Project\1_Logbook Generator\logbook-generator-web\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C6801DA-20BD-49C6-B097-25A03D9BF1C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB313F85-AE0B-4F80-A06D-A8A0B475CD22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -82,8 +82,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-13809]hh:mm;@"/>
+    <numFmt numFmtId="166" formatCode="[$-13809]dd/mm/yyyy;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -153,7 +154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -194,6 +195,9 @@
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,7 +504,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -546,7 +550,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+      <c r="A2" s="16">
         <v>45832</v>
       </c>
       <c r="B2" s="6" t="s">

</xml_diff>